<commit_message>
custom drop filter | custom radio button
</commit_message>
<xml_diff>
--- a/src/data/data.xlsx
+++ b/src/data/data.xlsx
@@ -4,55 +4,58 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20117" windowHeight="11614"/>
+    <workbookView windowWidth="24685" windowHeight="11614"/>
   </bookViews>
   <sheets>
     <sheet name="Yeni Metin Belgesi" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Yeni Metin Belgesi'!$A$1:$L$201</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="370">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>depo</t>
-  </si>
-  <si>
-    <t>sehir</t>
-  </si>
-  <si>
-    <t>bazdagilim</t>
-  </si>
-  <si>
-    <t>gunceldagilim</t>
-  </si>
-  <si>
-    <t>stok</t>
-  </si>
-  <si>
-    <t>siparis</t>
-  </si>
-  <si>
-    <t>hakedis</t>
-  </si>
-  <si>
-    <t>sip_hak_fark</t>
-  </si>
-  <si>
-    <t>gonderim</t>
-  </si>
-  <si>
-    <t>aysonustok</t>
-  </si>
-  <si>
-    <t>aysonusit</t>
-  </si>
-  <si>
-    <t>LVMH Fragrance Brands</t>
+    <t>warehouse</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>basedist</t>
+  </si>
+  <si>
+    <t>currentdist</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>allowance</t>
+  </si>
+  <si>
+    <t>ord-alw-diff</t>
+  </si>
+  <si>
+    <t>transfer</t>
+  </si>
+  <si>
+    <t>monthly-last-stock</t>
+  </si>
+  <si>
+    <t>monthly-last-sit</t>
+  </si>
+  <si>
+    <t>LVMH Fragrance Brands XLSX</t>
   </si>
   <si>
     <t>Shentong</t>
@@ -229,7 +232,7 @@
     <t>Excellium Pharmaceutical, Inc</t>
   </si>
   <si>
-    <t>Strasbourg</t>
+    <t>Turochak</t>
   </si>
   <si>
     <t>L. Perrigo Company</t>
@@ -253,27 +256,18 @@
     <t>Lil' Drug Store Products, Inc</t>
   </si>
   <si>
-    <t>Sumberkrajan</t>
-  </si>
-  <si>
     <t>0.02</t>
   </si>
   <si>
     <t>Physicians Total Care, Inc.</t>
   </si>
   <si>
-    <t>Gaplokan</t>
-  </si>
-  <si>
     <t>0.05</t>
   </si>
   <si>
     <t>Dr. Reddy's Laboratories Inc</t>
   </si>
   <si>
-    <t>Yangzhuang</t>
-  </si>
-  <si>
     <t>Midlothian Laboratories</t>
   </si>
   <si>
@@ -322,18 +316,9 @@
     <t>Elizabeth Arden, Inc</t>
   </si>
   <si>
-    <t>Waxi</t>
-  </si>
-  <si>
-    <t>Dole</t>
-  </si>
-  <si>
     <t>Ventura Corporation LTD</t>
   </si>
   <si>
-    <t>Dadap</t>
-  </si>
-  <si>
     <t>Torrent Pharmaceuticals Limited</t>
   </si>
   <si>
@@ -394,21 +379,12 @@
     <t>0.22</t>
   </si>
   <si>
-    <t>Mulyosari</t>
-  </si>
-  <si>
     <t>Dolgencorp, LLC</t>
   </si>
   <si>
-    <t>Guilhabreu</t>
-  </si>
-  <si>
     <t>State of Florida DOH Central Pharmacy</t>
   </si>
   <si>
-    <t>Gävle</t>
-  </si>
-  <si>
     <t>Merck Sharp &amp; Dohme Corp.</t>
   </si>
   <si>
@@ -460,21 +436,12 @@
     <t>Western Family Foods Inc</t>
   </si>
   <si>
-    <t>Lille</t>
-  </si>
-  <si>
     <t>Natureplex LLC</t>
   </si>
   <si>
-    <t>Xianshui</t>
-  </si>
-  <si>
     <t>Apotex Corp.</t>
   </si>
   <si>
-    <t>Shklo</t>
-  </si>
-  <si>
     <t>Accra-Pac, Inc.</t>
   </si>
   <si>
@@ -496,7 +463,7 @@
     <t>E. Fougera &amp; Co. a division of Fougera Pharmaceuticals Inc.</t>
   </si>
   <si>
-    <t>Fresnes</t>
+    <t>Ourozinho</t>
   </si>
   <si>
     <t>Hi-Tech Pharmacal Co., Inc.</t>
@@ -505,18 +472,9 @@
     <t>Modosinal</t>
   </si>
   <si>
-    <t>Iława</t>
-  </si>
-  <si>
     <t>Combe Incorporated</t>
   </si>
   <si>
-    <t>Nanqiao</t>
-  </si>
-  <si>
-    <t>Wu’erbu Baolige</t>
-  </si>
-  <si>
     <t>Walgreen</t>
   </si>
   <si>
@@ -541,9 +499,6 @@
     <t>Rogachëvo</t>
   </si>
   <si>
-    <t>Jiuchenggong</t>
-  </si>
-  <si>
     <t>Ruchihe</t>
   </si>
   <si>
@@ -580,15 +535,9 @@
     <t>Fushë-Bulqizë</t>
   </si>
   <si>
-    <t>Naranjo</t>
-  </si>
-  <si>
     <t>B. Braun Medical Inc.</t>
   </si>
   <si>
-    <t>Dalmacio Vélez Sársfield</t>
-  </si>
-  <si>
     <t>REMEDYREPACK INC.</t>
   </si>
   <si>
@@ -598,12 +547,6 @@
     <t>Rebel Distributors Corp</t>
   </si>
   <si>
-    <t>Waepana</t>
-  </si>
-  <si>
-    <t>Ribnica na Pohorju</t>
-  </si>
-  <si>
     <t>Kroger Company</t>
   </si>
   <si>
@@ -634,15 +577,9 @@
     <t>Watson Laboratories, Inc.</t>
   </si>
   <si>
-    <t>San Manuel Chaparrón</t>
-  </si>
-  <si>
     <t>Glenmark Generics Inc. USA</t>
   </si>
   <si>
-    <t>Wręczyca Wielka</t>
-  </si>
-  <si>
     <t>Walgreen Co</t>
   </si>
   <si>
@@ -718,9 +655,6 @@
     <t>Mankono</t>
   </si>
   <si>
-    <t>Ourozinho</t>
-  </si>
-  <si>
     <t>Lake Erie Medical &amp; Surgical Supply DBA Qualtiy Care Products LLC</t>
   </si>
   <si>
@@ -751,12 +685,6 @@
     <t>Shalizhai</t>
   </si>
   <si>
-    <t>Gierałtowice</t>
-  </si>
-  <si>
-    <t>Tegalgede Kulon</t>
-  </si>
-  <si>
     <t>Aurolife Pharma, LLC</t>
   </si>
   <si>
@@ -886,12 +814,6 @@
     <t>PSS World Medical, Inc.</t>
   </si>
   <si>
-    <t>Aconibe</t>
-  </si>
-  <si>
-    <t>Kocēni</t>
-  </si>
-  <si>
     <t>Perrigo New York Inc</t>
   </si>
   <si>
@@ -1084,15 +1006,9 @@
     <t>TYA Pharmaceuticals</t>
   </si>
   <si>
-    <t>Ban Talat Bueng</t>
-  </si>
-  <si>
     <t>Roxane Laboratories, Inc.</t>
   </si>
   <si>
-    <t>Sumuranyar</t>
-  </si>
-  <si>
     <t>AMOREPACIFIC</t>
   </si>
   <si>
@@ -1199,9 +1115,6 @@
   </si>
   <si>
     <t>Shache</t>
-  </si>
-  <si>
-    <t>Turochak</t>
   </si>
   <si>
     <t>McKesson Contract Packaging</t>
@@ -1221,12 +1134,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1240,6 +1153,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1258,8 +1184,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1268,6 +1195,14 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1286,6 +1221,13 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1336,22 +1278,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1365,9 +1292,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1375,13 +1301,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1396,13 +1315,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1414,55 +1387,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1480,37 +1411,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1523,30 +1436,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1576,7 +1465,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1587,6 +1506,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1661,44 +1606,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1710,130 +1629,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1844,8 +1763,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2169,46 +2088,51 @@
   <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.72972972972973" defaultRowHeight="14.55"/>
+  <cols>
+    <col min="2" max="2" width="33.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="24.7837837837838" customWidth="1"/>
+    <col min="12" max="12" width="14.5135135135135" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2980,10 +2904,10 @@
         <v>78</v>
       </c>
       <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
       </c>
       <c r="E22" t="s">
         <v>68</v>
@@ -3015,16 +2939,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
         <v>77</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F23">
         <v>1442</v>
@@ -3053,10 +2977,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -3091,10 +3015,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
         <v>55</v>
@@ -3129,10 +3053,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
         <v>55</v>
@@ -3167,10 +3091,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
@@ -3205,16 +3129,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F28">
         <v>2437</v>
@@ -3246,7 +3170,7 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>65</v>
@@ -3281,10 +3205,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
         <v>74</v>
@@ -3319,10 +3243,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
         <v>26</v>
@@ -3357,13 +3281,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
@@ -3395,10 +3319,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -3436,7 +3360,7 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
         <v>34</v>
@@ -3471,16 +3395,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
         <v>69</v>
       </c>
       <c r="E35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F35">
         <v>1689</v>
@@ -3509,10 +3433,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
         <v>62</v>
@@ -3547,10 +3471,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
         <v>22</v>
@@ -3585,10 +3509,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
         <v>51</v>
@@ -3623,13 +3547,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E39" t="s">
         <v>62</v>
@@ -3661,16 +3585,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
         <v>29</v>
       </c>
       <c r="E40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F40">
         <v>1497</v>
@@ -3702,7 +3626,7 @@
         <v>27</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D41" t="s">
         <v>68</v>
@@ -3737,10 +3661,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C42" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
         <v>54</v>
@@ -3775,16 +3699,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F43">
         <v>778</v>
@@ -3813,16 +3737,16 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E44" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F44">
         <v>1942</v>
@@ -3851,10 +3775,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
         <v>15</v>
@@ -3889,16 +3813,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
         <v>43</v>
       </c>
       <c r="E46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F46">
         <v>1448</v>
@@ -3927,10 +3851,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>130</v>
+        <v>71</v>
       </c>
       <c r="D47" t="s">
         <v>69</v>
@@ -3965,10 +3889,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C48" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="D48" t="s">
         <v>54</v>
@@ -4003,10 +3927,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C49" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D49" t="s">
         <v>33</v>
@@ -4041,10 +3965,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>
@@ -4079,16 +4003,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F51">
         <v>2888</v>
@@ -4117,10 +4041,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D52" t="s">
         <v>43</v>
@@ -4155,13 +4079,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
         <v>46</v>
@@ -4193,10 +4117,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
         <v>69</v>
@@ -4231,13 +4155,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
         <v>18</v>
@@ -4269,10 +4193,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="D56" t="s">
         <v>61</v>
@@ -4307,10 +4231,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="D57" t="s">
         <v>46</v>
@@ -4345,10 +4269,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
         <v>46</v>
@@ -4383,10 +4307,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C59" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D59" t="s">
         <v>40</v>
@@ -4421,10 +4345,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D60" t="s">
         <v>77</v>
@@ -4459,10 +4383,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D61" t="s">
         <v>23</v>
@@ -4497,10 +4421,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>159</v>
-      </c>
-      <c r="C62" t="s">
-        <v>160</v>
+        <v>147</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D62" t="s">
         <v>18</v>
@@ -4535,10 +4459,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C63" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s">
         <v>23</v>
@@ -4573,10 +4497,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
@@ -4611,10 +4535,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="C65" t="s">
-        <v>165</v>
+        <v>71</v>
       </c>
       <c r="D65" t="s">
         <v>34</v>
@@ -4652,7 +4576,7 @@
         <v>27</v>
       </c>
       <c r="C66" t="s">
-        <v>166</v>
+        <v>71</v>
       </c>
       <c r="D66" t="s">
         <v>33</v>
@@ -4687,10 +4611,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D67" t="s">
         <v>77</v>
@@ -4725,10 +4649,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="D68" t="s">
         <v>30</v>
@@ -4763,10 +4687,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D69" t="s">
         <v>61</v>
@@ -4801,10 +4725,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="D70" t="s">
         <v>54</v>
@@ -4839,16 +4763,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
-      </c>
-      <c r="C71" t="s">
-        <v>175</v>
+        <v>140</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D71" t="s">
         <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F71">
         <v>1460</v>
@@ -4880,7 +4804,7 @@
         <v>24</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D72" t="s">
         <v>54</v>
@@ -4915,13 +4839,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C73" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D73" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E73" t="s">
         <v>19</v>
@@ -4953,16 +4877,16 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C74" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D74" t="s">
         <v>65</v>
       </c>
       <c r="E74" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F74">
         <v>1550</v>
@@ -4991,10 +4915,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C75" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="D75" t="s">
         <v>33</v>
@@ -5029,10 +4953,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C76" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D76" t="s">
         <v>43</v>
@@ -5067,10 +4991,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C77" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D77" t="s">
         <v>54</v>
@@ -5105,10 +5029,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="D78" t="s">
         <v>30</v>
@@ -5146,7 +5070,7 @@
         <v>52</v>
       </c>
       <c r="C79" t="s">
-        <v>188</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
         <v>62</v>
@@ -5181,16 +5105,16 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="C80" t="s">
-        <v>190</v>
+        <v>71</v>
       </c>
       <c r="D80" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E80" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F80">
         <v>1575</v>
@@ -5219,10 +5143,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C81" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="D81" t="s">
         <v>46</v>
@@ -5257,13 +5181,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>193</v>
-      </c>
-      <c r="C82" t="s">
-        <v>194</v>
+        <v>175</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D82" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E82" t="s">
         <v>61</v>
@@ -5295,10 +5219,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>191</v>
-      </c>
-      <c r="C83" t="s">
-        <v>195</v>
+        <v>173</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D83" t="s">
         <v>58</v>
@@ -5333,10 +5257,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="C84" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="D84" t="s">
         <v>37</v>
@@ -5371,10 +5295,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="D85" t="s">
         <v>30</v>
@@ -5409,10 +5333,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C86" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D86" t="s">
         <v>30</v>
@@ -5447,10 +5371,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C87" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="D87" t="s">
         <v>58</v>
@@ -5485,16 +5409,16 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="C88" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="D88" t="s">
         <v>65</v>
       </c>
       <c r="E88" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F88">
         <v>2264</v>
@@ -5523,13 +5447,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>205</v>
-      </c>
-      <c r="C89" t="s">
-        <v>206</v>
+        <v>185</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D89" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E89" t="s">
         <v>61</v>
@@ -5561,10 +5485,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>207</v>
-      </c>
-      <c r="C90" t="s">
-        <v>208</v>
+        <v>186</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D90" t="s">
         <v>30</v>
@@ -5599,10 +5523,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="C91" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="D91" t="s">
         <v>19</v>
@@ -5637,16 +5561,16 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="C92" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D92" t="s">
         <v>19</v>
       </c>
       <c r="E92" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F92">
         <v>2823</v>
@@ -5675,16 +5599,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="C93" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="D93" t="s">
         <v>65</v>
       </c>
       <c r="E93" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F93">
         <v>578</v>
@@ -5713,13 +5637,13 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="D94" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E94" t="s">
         <v>22</v>
@@ -5751,10 +5675,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="C95" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -5789,10 +5713,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="D96" t="s">
         <v>15</v>
@@ -5827,10 +5751,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>220</v>
+        <v>198</v>
       </c>
       <c r="C97" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="D97" t="s">
         <v>37</v>
@@ -5865,13 +5789,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="C98" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
       <c r="D98" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E98" t="s">
         <v>51</v>
@@ -5903,10 +5827,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>224</v>
+        <v>202</v>
       </c>
       <c r="C99" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="D99" t="s">
         <v>54</v>
@@ -5941,16 +5865,16 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>226</v>
+        <v>204</v>
       </c>
       <c r="C100" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="D100" t="s">
         <v>23</v>
       </c>
       <c r="E100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F100">
         <v>770</v>
@@ -5979,10 +5903,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C101" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
       <c r="D101" t="s">
         <v>69</v>
@@ -6017,13 +5941,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>229</v>
+        <v>207</v>
       </c>
       <c r="C102" t="s">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="D102" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E102" t="s">
         <v>43</v>
@@ -6055,10 +5979,10 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="C103" t="s">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="D103" t="s">
         <v>43</v>
@@ -6093,10 +6017,10 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C104" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="D104" t="s">
         <v>46</v>
@@ -6134,10 +6058,10 @@
         <v>75</v>
       </c>
       <c r="C105" t="s">
-        <v>234</v>
+        <v>148</v>
       </c>
       <c r="D105" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E105" t="s">
         <v>18</v>
@@ -6169,10 +6093,10 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="C106" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="D106" t="s">
         <v>58</v>
@@ -6207,13 +6131,13 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="C107" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="D107" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E107" t="s">
         <v>26</v>
@@ -6248,7 +6172,7 @@
         <v>16</v>
       </c>
       <c r="C108" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="D108" t="s">
         <v>54</v>
@@ -6283,10 +6207,10 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="C109" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="D109" t="s">
         <v>54</v>
@@ -6321,16 +6245,16 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="C110" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="D110" t="s">
         <v>54</v>
       </c>
       <c r="E110" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F110">
         <v>956</v>
@@ -6359,16 +6283,16 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="C111" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="D111" t="s">
         <v>55</v>
       </c>
       <c r="E111" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F111">
         <v>1932</v>
@@ -6397,13 +6321,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>143</v>
-      </c>
-      <c r="C112" t="s">
-        <v>245</v>
+        <v>134</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D112" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E112" t="s">
         <v>22</v>
@@ -6435,16 +6359,16 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>191</v>
-      </c>
-      <c r="C113" t="s">
-        <v>246</v>
+        <v>173</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D113" t="s">
         <v>34</v>
       </c>
       <c r="E113" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F113">
         <v>2560</v>
@@ -6473,10 +6397,10 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="C114" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="D114" t="s">
         <v>46</v>
@@ -6511,10 +6435,10 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="C115" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
       <c r="D115" t="s">
         <v>69</v>
@@ -6549,10 +6473,10 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="C116" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="D116" t="s">
         <v>15</v>
@@ -6587,10 +6511,10 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C117" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="D117" t="s">
         <v>33</v>
@@ -6625,16 +6549,16 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="C118" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="D118" t="s">
         <v>69</v>
       </c>
       <c r="E118" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F118">
         <v>1992</v>
@@ -6666,7 +6590,7 @@
         <v>75</v>
       </c>
       <c r="C119" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -6701,16 +6625,16 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="C120" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="D120" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E120" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F120">
         <v>1976</v>
@@ -6739,10 +6663,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="C121" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="D121" t="s">
         <v>19</v>
@@ -6777,10 +6701,10 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="C122" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="D122" t="s">
         <v>58</v>
@@ -6815,16 +6739,16 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C123" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="D123" t="s">
         <v>36</v>
       </c>
       <c r="E123" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F123">
         <v>2723</v>
@@ -6853,10 +6777,10 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="C124" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="D124" t="s">
         <v>43</v>
@@ -6891,16 +6815,16 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="C125" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="D125" t="s">
         <v>69</v>
       </c>
       <c r="E125" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F125">
         <v>1514</v>
@@ -6929,10 +6853,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="C126" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="D126" t="s">
         <v>15</v>
@@ -6967,10 +6891,10 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="C127" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="D127" t="s">
         <v>55</v>
@@ -7005,10 +6929,10 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="C128" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="D128" t="s">
         <v>65</v>
@@ -7043,13 +6967,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>272</v>
+        <v>247</v>
       </c>
       <c r="C129" t="s">
-        <v>273</v>
+        <v>248</v>
       </c>
       <c r="D129" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E129" t="s">
         <v>77</v>
@@ -7081,16 +7005,16 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="C130" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="D130" t="s">
         <v>40</v>
       </c>
       <c r="E130" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F130">
         <v>1903</v>
@@ -7119,10 +7043,10 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="C131" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="D131" t="s">
         <v>69</v>
@@ -7157,16 +7081,16 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="C132" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="D132" t="s">
         <v>30</v>
       </c>
       <c r="E132" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F132">
         <v>1342</v>
@@ -7195,16 +7119,16 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="C133" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="D133" t="s">
         <v>29</v>
       </c>
       <c r="E133" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F133">
         <v>1335</v>
@@ -7233,10 +7157,10 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="C134" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="D134" t="s">
         <v>19</v>
@@ -7274,13 +7198,13 @@
         <v>66</v>
       </c>
       <c r="C135" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="D135" t="s">
         <v>43</v>
       </c>
       <c r="E135" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F135">
         <v>1941</v>
@@ -7309,13 +7233,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="C136" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="D136" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E136" t="s">
         <v>61</v>
@@ -7347,16 +7271,16 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C137" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="D137" t="s">
         <v>55</v>
       </c>
       <c r="E137" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F137">
         <v>2295</v>
@@ -7385,10 +7309,10 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="C138" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="D138" t="s">
         <v>33</v>
@@ -7423,10 +7347,10 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C139" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="D139" t="s">
         <v>55</v>
@@ -7461,10 +7385,10 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>289</v>
-      </c>
-      <c r="C140" t="s">
-        <v>290</v>
+        <v>264</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D140" t="s">
         <v>58</v>
@@ -7501,8 +7425,8 @@
       <c r="B141" t="s">
         <v>47</v>
       </c>
-      <c r="C141" t="s">
-        <v>291</v>
+      <c r="C141" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D141" t="s">
         <v>43</v>
@@ -7537,10 +7461,10 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="C142" t="s">
-        <v>293</v>
+        <v>266</v>
       </c>
       <c r="D142" t="s">
         <v>62</v>
@@ -7575,10 +7499,10 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="C143" t="s">
-        <v>295</v>
+        <v>268</v>
       </c>
       <c r="D143" t="s">
         <v>23</v>
@@ -7613,16 +7537,16 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="C144" t="s">
-        <v>297</v>
+        <v>270</v>
       </c>
       <c r="D144" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E144" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F144">
         <v>1903</v>
@@ -7651,10 +7575,10 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>298</v>
+        <v>271</v>
       </c>
       <c r="C145" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="D145" t="s">
         <v>34</v>
@@ -7689,10 +7613,10 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="C146" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
       <c r="D146" t="s">
         <v>19</v>
@@ -7727,16 +7651,16 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C147" t="s">
-        <v>302</v>
+        <v>275</v>
       </c>
       <c r="D147" t="s">
         <v>62</v>
       </c>
       <c r="E147" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F147">
         <v>2611</v>
@@ -7765,10 +7689,10 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>303</v>
+        <v>276</v>
       </c>
       <c r="C148" t="s">
-        <v>304</v>
+        <v>277</v>
       </c>
       <c r="D148" t="s">
         <v>40</v>
@@ -7803,16 +7727,16 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="C149" t="s">
-        <v>306</v>
+        <v>279</v>
       </c>
       <c r="D149" t="s">
         <v>61</v>
       </c>
       <c r="E149" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F149">
         <v>2005</v>
@@ -7841,10 +7765,10 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>307</v>
+        <v>280</v>
       </c>
       <c r="C150" t="s">
-        <v>308</v>
+        <v>281</v>
       </c>
       <c r="D150" t="s">
         <v>29</v>
@@ -7879,16 +7803,16 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>309</v>
+        <v>282</v>
       </c>
       <c r="C151" t="s">
-        <v>310</v>
+        <v>283</v>
       </c>
       <c r="D151" t="s">
         <v>74</v>
       </c>
       <c r="E151" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F151">
         <v>2723</v>
@@ -7917,16 +7841,16 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>311</v>
+        <v>284</v>
       </c>
       <c r="C152" t="s">
-        <v>312</v>
+        <v>285</v>
       </c>
       <c r="D152" t="s">
         <v>30</v>
       </c>
       <c r="E152" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F152">
         <v>773</v>
@@ -7955,10 +7879,10 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>313</v>
+        <v>286</v>
       </c>
       <c r="C153" t="s">
-        <v>314</v>
+        <v>287</v>
       </c>
       <c r="D153" t="s">
         <v>18</v>
@@ -7993,13 +7917,13 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="C154" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="D154" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E154" t="s">
         <v>33</v>
@@ -8031,16 +7955,16 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>316</v>
+        <v>289</v>
       </c>
       <c r="C155" t="s">
-        <v>317</v>
+        <v>290</v>
       </c>
       <c r="D155" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E155" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F155">
         <v>1813</v>
@@ -8069,10 +7993,10 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>318</v>
+        <v>291</v>
       </c>
       <c r="C156" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="D156" t="s">
         <v>19</v>
@@ -8107,10 +8031,10 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>320</v>
+        <v>293</v>
       </c>
       <c r="C157" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="D157" t="s">
         <v>19</v>
@@ -8145,10 +8069,10 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C158" t="s">
-        <v>322</v>
+        <v>295</v>
       </c>
       <c r="D158" t="s">
         <v>26</v>
@@ -8183,13 +8107,13 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="C159" t="s">
-        <v>323</v>
+        <v>296</v>
       </c>
       <c r="D159" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E159" t="s">
         <v>61</v>
@@ -8221,10 +8145,10 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>324</v>
+        <v>297</v>
       </c>
       <c r="C160" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="D160" t="s">
         <v>68</v>
@@ -8259,10 +8183,10 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>326</v>
+        <v>299</v>
       </c>
       <c r="C161" t="s">
-        <v>327</v>
+        <v>300</v>
       </c>
       <c r="D161" t="s">
         <v>36</v>
@@ -8300,7 +8224,7 @@
         <v>75</v>
       </c>
       <c r="C162" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="D162" t="s">
         <v>55</v>
@@ -8335,10 +8259,10 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C163" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="D163" t="s">
         <v>43</v>
@@ -8373,10 +8297,10 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="C164" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="D164" t="s">
         <v>23</v>
@@ -8411,10 +8335,10 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="C165" t="s">
-        <v>333</v>
+        <v>306</v>
       </c>
       <c r="D165" t="s">
         <v>40</v>
@@ -8449,13 +8373,13 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
       <c r="C166" t="s">
-        <v>335</v>
+        <v>308</v>
       </c>
       <c r="D166" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E166" t="s">
         <v>62</v>
@@ -8487,10 +8411,10 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="C167" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="D167" t="s">
         <v>69</v>
@@ -8525,16 +8449,16 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="C168" t="s">
-        <v>339</v>
+        <v>312</v>
       </c>
       <c r="D168" t="s">
         <v>77</v>
       </c>
       <c r="E168" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F168">
         <v>81</v>
@@ -8563,13 +8487,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>340</v>
+        <v>313</v>
       </c>
       <c r="C169" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="D169" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E169" t="s">
         <v>43</v>
@@ -8604,7 +8528,7 @@
         <v>27</v>
       </c>
       <c r="C170" t="s">
-        <v>342</v>
+        <v>315</v>
       </c>
       <c r="D170" t="s">
         <v>65</v>
@@ -8639,10 +8563,10 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="C171" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="D171" t="s">
         <v>29</v>
@@ -8677,16 +8601,16 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="C172" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="D172" t="s">
         <v>34</v>
       </c>
       <c r="E172" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F172">
         <v>2722</v>
@@ -8715,10 +8639,10 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="C173" t="s">
-        <v>348</v>
+        <v>321</v>
       </c>
       <c r="D173" t="s">
         <v>22</v>
@@ -8753,10 +8677,10 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="C174" t="s">
-        <v>350</v>
+        <v>323</v>
       </c>
       <c r="D174" t="s">
         <v>40</v>
@@ -8791,10 +8715,10 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>351</v>
+        <v>324</v>
       </c>
       <c r="C175" t="s">
-        <v>352</v>
+        <v>325</v>
       </c>
       <c r="D175" t="s">
         <v>15</v>
@@ -8832,7 +8756,7 @@
         <v>16</v>
       </c>
       <c r="C176" t="s">
-        <v>353</v>
+        <v>326</v>
       </c>
       <c r="D176" t="s">
         <v>15</v>
@@ -8867,16 +8791,16 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="C177" t="s">
-        <v>354</v>
+        <v>327</v>
       </c>
       <c r="D177" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E177" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F177">
         <v>1968</v>
@@ -8905,16 +8829,16 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>355</v>
-      </c>
-      <c r="C178" t="s">
-        <v>356</v>
+        <v>328</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D178" t="s">
         <v>54</v>
       </c>
       <c r="E178" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="F178">
         <v>1312</v>
@@ -8943,10 +8867,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>357</v>
-      </c>
-      <c r="C179" t="s">
-        <v>358</v>
+        <v>329</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="D179" t="s">
         <v>30</v>
@@ -8981,10 +8905,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="C180" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
       <c r="D180" t="s">
         <v>22</v>
@@ -9019,10 +8943,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
       <c r="C181" t="s">
-        <v>362</v>
+        <v>333</v>
       </c>
       <c r="D181" t="s">
         <v>65</v>
@@ -9057,10 +8981,10 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
       <c r="C182" t="s">
-        <v>364</v>
+        <v>335</v>
       </c>
       <c r="D182" t="s">
         <v>55</v>
@@ -9095,10 +9019,10 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
       <c r="C183" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
       <c r="D183" t="s">
         <v>22</v>
@@ -9133,10 +9057,10 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
       <c r="C184" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="D184" t="s">
         <v>51</v>
@@ -9171,10 +9095,10 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="C185" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="D185" t="s">
         <v>33</v>
@@ -9209,10 +9133,10 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>305</v>
+        <v>278</v>
       </c>
       <c r="C186" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="D186" t="s">
         <v>40</v>
@@ -9247,10 +9171,10 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="C187" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="D187" t="s">
         <v>23</v>
@@ -9285,13 +9209,13 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
       <c r="C188" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="D188" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E188" t="s">
         <v>37</v>
@@ -9323,10 +9247,10 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="C189" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="D189" t="s">
         <v>34</v>
@@ -9361,10 +9285,10 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="C190" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="D190" t="s">
         <v>30</v>
@@ -9399,10 +9323,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="C191" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
       <c r="D191" t="s">
         <v>15</v>
@@ -9437,10 +9361,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
       <c r="C192" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
       <c r="D192" t="s">
         <v>61</v>
@@ -9475,10 +9399,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
       <c r="C193" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
       <c r="D193" t="s">
         <v>14</v>
@@ -9513,10 +9437,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>386</v>
+        <v>357</v>
       </c>
       <c r="C194" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
       <c r="D194" t="s">
         <v>77</v>
@@ -9551,10 +9475,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
       <c r="C195" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
       <c r="D195" t="s">
         <v>30</v>
@@ -9589,10 +9513,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>390</v>
+        <v>361</v>
       </c>
       <c r="C196" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
       <c r="D196" t="s">
         <v>37</v>
@@ -9627,16 +9551,16 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>392</v>
+        <v>363</v>
       </c>
       <c r="C197" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
       <c r="D197" t="s">
         <v>68</v>
       </c>
       <c r="E197" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F197">
         <v>2873</v>
@@ -9665,10 +9589,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C198" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
       <c r="D198" t="s">
         <v>54</v>
@@ -9703,10 +9627,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C199" t="s">
-        <v>395</v>
+        <v>71</v>
       </c>
       <c r="D199" t="s">
         <v>29</v>
@@ -9741,10 +9665,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="C200" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
       <c r="D200" t="s">
         <v>18</v>
@@ -9779,13 +9703,13 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
       <c r="C201" t="s">
-        <v>399</v>
+        <v>369</v>
       </c>
       <c r="D201" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E201" t="s">
         <v>34</v>
@@ -9813,6 +9737,9 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L201">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>